<commit_message>
Removed seed randomizer and added Archipelago client
</commit_message>
<xml_diff>
--- a/LevelDumps/ItemLocations.xlsx
+++ b/LevelDumps/ItemLocations.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hoila\source\repos\TunicRandomizer\LevelDumps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{144989C3-EADE-489A-BC06-CAFB6B7F4C58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEC291ED-4EB4-4AD4-85A3-39BD64896B05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$O$267</definedName>
+  </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
@@ -4009,7 +4012,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H18" sqref="H18"/>
+      <selection pane="bottomLeft" activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15534,6 +15537,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:O267" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>